<commit_message>
Add new feature to print recap attendance for trainer, individually - per class - aggregate
</commit_message>
<xml_diff>
--- a/file/template/pusdiklat/execution/STANDAR_REKAPITULASI_KEHADIRAN_PESERTA_DIKLAT.xlsx
+++ b/file/template/pusdiklat/execution/STANDAR_REKAPITULASI_KEHADIRAN_PESERTA_DIKLAT.xlsx
@@ -15,13 +15,15 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Rekap Kehadiran Peserta'!$A$1:$I$17</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Rekap Kehadiran Peserta'!$A$1:$I$17</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Rekap Kehadiran Peserta'!$A$1:$I$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Rekap Kehadiran Peserta'!$A$1:$I$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Rekap Kehadiran Peserta'!$A$1:$I$17</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>REKAPITULASI KEHADIRAN PESERTA</t>
   </si>
@@ -77,55 +79,7 @@
     <t>Jakarta,         Mei 2014</t>
   </si>
   <si>
-    <t>Crmh 1</t>
-  </si>
-  <si>
-    <t>Ceramah Current Issue</t>
-  </si>
-  <si>
-    <t>MP 3</t>
-  </si>
-  <si>
-    <t>Teknik Penyusunan BAP dan Pemberkasan</t>
-  </si>
-  <si>
     <t>Kepala Bidang Penyelenggaraan</t>
-  </si>
-  <si>
-    <t>MP 1</t>
-  </si>
-  <si>
-    <t>Overview PP No.  Tahun  dan Juklak (Petunjuk Pelaksanaan)</t>
-  </si>
-  <si>
-    <t>MP 4</t>
-  </si>
-  <si>
-    <t>Teknik Penyusunan Laporan Hasil Pemeriksaan</t>
-  </si>
-  <si>
-    <t>MP 2</t>
-  </si>
-  <si>
-    <t>Teknik-teknik Pemeriksaan</t>
-  </si>
-  <si>
-    <t>MP 5</t>
-  </si>
-  <si>
-    <t>Studi Kasus Komprehensif</t>
-  </si>
-  <si>
-    <t>Crmh 2</t>
-  </si>
-  <si>
-    <t>Ceramah Capacity Building</t>
-  </si>
-  <si>
-    <t>Crmh 3</t>
-  </si>
-  <si>
-    <t>Ceramah Soft Competency  Integritas  Anti Korupsi</t>
   </si>
   <si>
     <t>Hercarmina</t>
@@ -427,15 +381,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>214200</xdr:colOff>
+      <xdr:colOff>268200</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>503280</xdr:colOff>
+      <xdr:colOff>556560</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>47520</xdr:rowOff>
+      <xdr:rowOff>46800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -450,8 +404,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="214200" y="0"/>
-          <a:ext cx="732240" cy="618840"/>
+          <a:off x="268200" y="0"/>
+          <a:ext cx="731520" cy="618120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -475,7 +429,7 @@
   <dimension ref="1:17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9:I9"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -650,79 +604,47 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="17"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="A13" s="17"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="17"/>
-      <c r="D13" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>26</v>
-      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="16"/>
       <c r="F13" s="19"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>28</v>
-      </c>
+      <c r="A14" s="17"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="17"/>
-      <c r="D14" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>30</v>
-      </c>
+      <c r="D14" s="17"/>
+      <c r="E14" s="16"/>
       <c r="F14" s="19"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>32</v>
-      </c>
+      <c r="A15" s="17"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="17"/>
-      <c r="D15" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>34</v>
-      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="16"/>
       <c r="F15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F16" s="20" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F17" s="18" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>